<commit_message>
update file sinkronisasi data dan ekspor to sql
</commit_message>
<xml_diff>
--- a/Latihan/data_source/depo.xlsx
+++ b/Latihan/data_source/depo.xlsx
@@ -1,28 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="600" windowWidth="13095" windowHeight="11190"/>
+    <workbookView windowWidth="20490" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="depo" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">depo!$A$1:$H$1</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="125725" forceFullCalc="1"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="100">
   <si>
     <t>DAOP 1 JAKARTA</t>
   </si>
   <si>
-    <t>Depo Lokomotif Tanah Abang</t>
+    <t>Depo Lokomotif THB</t>
   </si>
   <si>
     <t>PT Kereta Api Indonesia (Persero)</t>
@@ -31,22 +33,22 @@
     <t>Depo Sarana Penggerak</t>
   </si>
   <si>
-    <t>Depo Lokomotif Jatinegara</t>
-  </si>
-  <si>
-    <t>Depo Kereta Jakarta Kota</t>
+    <t>Depo Lokomotif CPN</t>
+  </si>
+  <si>
+    <t>Depo Kereta JAKK</t>
   </si>
   <si>
     <t>Depo Sarana Tanpa Penggerak</t>
   </si>
   <si>
-    <t>Depo Gerbong Jakarta Gudang</t>
-  </si>
-  <si>
-    <t>Depo Kereta Rangkas Bitung</t>
-  </si>
-  <si>
-    <t>Depo Kereta Jakarta Manggarai</t>
+    <t>Depo Gerbong JAKG</t>
+  </si>
+  <si>
+    <t>Depo Kereta RK</t>
+  </si>
+  <si>
+    <t>Depo Kereta JAKRI</t>
   </si>
   <si>
     <t>DEPO KRL MANGGARAI</t>
@@ -61,28 +63,28 @@
     <t>DAOP 2 BANDUNG</t>
   </si>
   <si>
-    <t>Depo Lokomotif Bandung</t>
-  </si>
-  <si>
-    <t>Depo Kereta / KRD Bandung</t>
+    <t>Depo Lokomotif BD</t>
+  </si>
+  <si>
+    <t>Depo Kereta BD</t>
   </si>
   <si>
     <t>DAOP 3 CIREBON</t>
   </si>
   <si>
-    <t>Depo Lokomotif Cirebon</t>
-  </si>
-  <si>
-    <t>Depo Kereta Cirebon</t>
+    <t>Depo Lokomotif CN</t>
+  </si>
+  <si>
+    <t>Depo Kereta CN</t>
   </si>
   <si>
     <t>DAOP 4 SEMARANG</t>
   </si>
   <si>
-    <t>Depo Lokomotif Semarang Poncol</t>
-  </si>
-  <si>
-    <t>Depo Kereta Semarang Poncol</t>
+    <t>Depo Lokomotif SMC</t>
+  </si>
+  <si>
+    <t>Depo Kereta SMC</t>
   </si>
   <si>
     <t>Depo Kereta Cepu</t>
@@ -94,16 +96,16 @@
     <t>DAOP 5 PURWOKERTO</t>
   </si>
   <si>
-    <t>Depo Lokomotif Purwokerto</t>
-  </si>
-  <si>
-    <t>Depo Kereta Purwokerto</t>
-  </si>
-  <si>
-    <t>Depo Kereta Kutoarjo</t>
-  </si>
-  <si>
-    <t>Depo Gerbong Maos</t>
+    <t>Depo Lokomotif PWT</t>
+  </si>
+  <si>
+    <t>Depo Kereta PWT</t>
+  </si>
+  <si>
+    <t>Depo Kereta KTA</t>
+  </si>
+  <si>
+    <t>Depo Gerbong MA</t>
   </si>
   <si>
     <t>Depo Lokomotif Cilacap</t>
@@ -115,16 +117,16 @@
     <t>DAOP 6 YOGYAKARTA</t>
   </si>
   <si>
-    <t>Depo Lokomotif Yogyakarta</t>
-  </si>
-  <si>
-    <t>Depo Kereta Yogyakarta</t>
-  </si>
-  <si>
-    <t>Depo Lokomotif Solo</t>
-  </si>
-  <si>
-    <t>Depo Kereta Solo</t>
+    <t>Depo Lokomotif YK</t>
+  </si>
+  <si>
+    <t>Depo Kereta YK</t>
+  </si>
+  <si>
+    <t>Depo Lokomotif SLO</t>
+  </si>
+  <si>
+    <t>Depo Kereta SLO</t>
   </si>
   <si>
     <t>Depo Mekanik Purwosari</t>
@@ -133,58 +135,58 @@
     <t>DAOP 7 MADIUN</t>
   </si>
   <si>
-    <t>Depo Lokomotif Madiun</t>
-  </si>
-  <si>
-    <t>Depo Kereta Madiun</t>
-  </si>
-  <si>
-    <t>Depo Mekanik Madiun</t>
+    <t>Depo Lokomotif MN</t>
+  </si>
+  <si>
+    <t>Depo Kereta BL</t>
+  </si>
+  <si>
+    <t>Depo Mekanik MN</t>
   </si>
   <si>
     <t>DAOP 8 SURABAYA</t>
   </si>
   <si>
-    <t>Depo Lokomotif Sidotopo</t>
-  </si>
-  <si>
-    <t>Depo Kereta / KRD Sidotopo</t>
-  </si>
-  <si>
-    <t>Depo Kereta Surabaya Pasar Turi</t>
+    <t>Depo Lokomotif SDT</t>
+  </si>
+  <si>
+    <t>Depo Kereta SDT</t>
+  </si>
+  <si>
+    <t>Depo Kereta SBI</t>
   </si>
   <si>
     <t>Depo Kereta Surabaya Gubeng</t>
   </si>
   <si>
-    <t>Depo Lokomotif Malang</t>
-  </si>
-  <si>
-    <t>Depo Kereta Malang</t>
-  </si>
-  <si>
-    <t>Depo Gerbong Sidotopo</t>
+    <t>Depo Lokomotif ML</t>
+  </si>
+  <si>
+    <t>Depo Kereta ML</t>
+  </si>
+  <si>
+    <t>Depo Gerbong SDT</t>
   </si>
   <si>
     <t>DAOP 9 JEMBER</t>
   </si>
   <si>
-    <t>Depo Lokomotif Jember</t>
-  </si>
-  <si>
-    <t>Depo Kereta Banyuwangi</t>
+    <t>Depo Lokomotif JR</t>
+  </si>
+  <si>
+    <t>Depo Kereta BW</t>
   </si>
   <si>
     <t>DIVRE I SUMATERA UTARA</t>
   </si>
   <si>
-    <t>Depo Lokomotif Medan</t>
-  </si>
-  <si>
-    <t>Depo Kereta Medan</t>
-  </si>
-  <si>
-    <t>Railink - Sumatera Utara</t>
+    <t>Depo Lokomotif MDN</t>
+  </si>
+  <si>
+    <t>Depo Kereta MDN</t>
+  </si>
+  <si>
+    <t>Depo KRD MDN</t>
   </si>
   <si>
     <t>Depo Kereta Aceh</t>
@@ -196,22 +198,22 @@
     <t>DIVRE II SUMATERA BARAT</t>
   </si>
   <si>
-    <t>Depo Lokomotif Padang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Depo Kereta Padang </t>
+    <t>Depo Lokomotif PD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depo Kereta PD </t>
   </si>
   <si>
     <t>DIVRE III SUMATERA SELATAN</t>
   </si>
   <si>
-    <t>Depo Lokomotif Kertapati</t>
-  </si>
-  <si>
-    <t>Depo Kereta Kertapati</t>
-  </si>
-  <si>
-    <t>Depo Gerbong Kertapati</t>
+    <t>Depo Lokomotif KPT</t>
+  </si>
+  <si>
+    <t>Depo Kereta KPT</t>
+  </si>
+  <si>
+    <t>Depo Gerbong KPT</t>
   </si>
   <si>
     <t>Depo Lokomotif Tanjung Enim Baru</t>
@@ -220,13 +222,13 @@
     <t>Depo Gerbong Tanjung Enim Baru</t>
   </si>
   <si>
-    <t>DEPO JAKABARING</t>
+    <t>DEPO LRT JAKABARING</t>
   </si>
   <si>
     <t>PT KAI COMMUTER JABOTABEK</t>
   </si>
   <si>
-    <t>Depo KRL Bukit Duri</t>
+    <t>Depo KRL BukitDuri</t>
   </si>
   <si>
     <t>Depo KRL Depok</t>
@@ -244,68 +246,445 @@
     <t>DIVRE IV LAMPUNG</t>
   </si>
   <si>
-    <t>Depo Lokomotif Tarahan</t>
-  </si>
-  <si>
-    <t>Depo Kereta Tanjung Karang</t>
-  </si>
-  <si>
-    <t>Depo Lokomotif Rejosari</t>
-  </si>
-  <si>
-    <t>Depo Kereta Rejosari</t>
-  </si>
-  <si>
-    <t>Depo Gerbong Rejosari</t>
-  </si>
-  <si>
-    <t>Depo Lokomotif Tanjung Karang</t>
-  </si>
-  <si>
-    <t>Depo Gerbong Tarahan</t>
+    <t>Depo Lokomotif THN</t>
+  </si>
+  <si>
+    <t>Depo Kereta TNK</t>
+  </si>
+  <si>
+    <t>Depo Lokomotif RJS</t>
+  </si>
+  <si>
+    <t>Depo Kereta RJS</t>
+  </si>
+  <si>
+    <t>Depo Gerbong RJS</t>
+  </si>
+  <si>
+    <t>Depo Lokomotif TNK</t>
+  </si>
+  <si>
+    <t>Depo Gerbong THN</t>
   </si>
   <si>
     <t>PROV DKI JAKARTA</t>
   </si>
   <si>
-    <t>Depo MRT Lebak Bulus</t>
+    <t>Depo MRT LebakBulus</t>
   </si>
   <si>
     <t>PT MRT Jakarta</t>
   </si>
   <si>
-    <t>DEPO KELAPA GADING</t>
+    <t>DEPO LRT KELAPAGADING</t>
   </si>
   <si>
     <t>PT LRT Jakarta</t>
   </si>
   <si>
-    <t>Depo APMS Bandara Soetta</t>
+    <t>Depo APMS BandaraSoetta</t>
   </si>
   <si>
     <t>PT Angkasa Pura II</t>
+  </si>
+  <si>
+    <t>Depo Gerbong AWN</t>
+  </si>
+  <si>
+    <t>DEPO GERBONG RWL</t>
+  </si>
+  <si>
+    <t>DEPO GERBONG BKP</t>
+  </si>
+  <si>
+    <t>Depo Gerbong SIG</t>
+  </si>
+  <si>
+    <t>DEPO GERBONG MRL</t>
+  </si>
+  <si>
+    <t>tambah depo baru</t>
+  </si>
+  <si>
+    <t>Daop 3</t>
+  </si>
+  <si>
+    <t>DAOP 6</t>
+  </si>
+  <si>
+    <t>Divre 2</t>
+  </si>
+  <si>
+    <t>Divre 3</t>
+  </si>
+  <si>
+    <t>Depo Gerbong Simpang</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -313,24 +692,315 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
         <i val="0"/>
       </font>
       <fill>
-        <patternFill>
+        <patternFill patternType="solid">
           <bgColor rgb="FFD7D7D7"/>
         </patternFill>
       </fill>
@@ -341,9 +1011,7 @@
         <i val="0"/>
       </font>
       <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
+        <patternFill patternType="none"/>
       </fill>
     </dxf>
   </dxfs>
@@ -353,6 +1021,11 @@
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -637,24 +1310,24 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H65"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
-    <col min="2" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="32.5714285714286" customWidth="1"/>
+    <col min="4" max="4" width="31.4285714285714" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -674,10 +1347,10 @@
         <v>3</v>
       </c>
       <c r="G1">
-        <v>-6.1841710000000001</v>
+        <v>-6.184171</v>
       </c>
       <c r="H1">
-        <v>106.81080799999999</v>
+        <v>106.810808</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -720,7 +1393,7 @@
         <v>6</v>
       </c>
       <c r="G3">
-        <v>-6.1346340000000001</v>
+        <v>-6.134634</v>
       </c>
       <c r="H3">
         <v>106.823285</v>
@@ -743,7 +1416,7 @@
         <v>6</v>
       </c>
       <c r="G4">
-        <v>-6.1333010000000003</v>
+        <v>-6.133301</v>
       </c>
       <c r="H4">
         <v>106.818028</v>
@@ -772,7 +1445,7 @@
         <v>106.253297</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>67</v>
       </c>
@@ -789,7 +1462,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>72</v>
       </c>
@@ -806,7 +1479,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>79</v>
       </c>
@@ -840,7 +1513,7 @@
         <v>3</v>
       </c>
       <c r="G9">
-        <v>-6.9133899999999997</v>
+        <v>-6.91339</v>
       </c>
       <c r="H9">
         <v>107.599592</v>
@@ -863,7 +1536,7 @@
         <v>6</v>
       </c>
       <c r="G10">
-        <v>-6.9139660000000003</v>
+        <v>-6.913966</v>
       </c>
       <c r="H10">
         <v>107.594613</v>
@@ -886,10 +1559,10 @@
         <v>3</v>
       </c>
       <c r="G11">
-        <v>-6.7033740000000002</v>
+        <v>-6.703374</v>
       </c>
       <c r="H11">
-        <v>108.55419000000001</v>
+        <v>108.55419</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -909,10 +1582,10 @@
         <v>6</v>
       </c>
       <c r="G12">
-        <v>-6.7063059999999997</v>
+        <v>-6.706306</v>
       </c>
       <c r="H12">
-        <v>108.55526999999999</v>
+        <v>108.55527</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -932,7 +1605,7 @@
         <v>3</v>
       </c>
       <c r="G13">
-        <v>-6.9729140000000003</v>
+        <v>-6.972914</v>
       </c>
       <c r="H13">
         <v>110.414699</v>
@@ -955,7 +1628,7 @@
         <v>6</v>
       </c>
       <c r="G14">
-        <v>-6.9733280000000004</v>
+        <v>-6.973328</v>
       </c>
       <c r="H14">
         <v>110.413516</v>
@@ -978,13 +1651,13 @@
         <v>6</v>
       </c>
       <c r="G15">
-        <v>-7.1558279999999996</v>
+        <v>-7.155828</v>
       </c>
       <c r="H15">
-        <v>111.58802799999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>111.588028</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>69</v>
       </c>
@@ -1041,7 +1714,7 @@
         <v>6</v>
       </c>
       <c r="G18">
-        <v>-7.4173070000000001</v>
+        <v>-7.417307</v>
       </c>
       <c r="H18">
         <v>109.221189</v>
@@ -1064,7 +1737,7 @@
         <v>6</v>
       </c>
       <c r="G19">
-        <v>-7.7264619999999997</v>
+        <v>-7.726462</v>
       </c>
       <c r="H19">
         <v>109.909499</v>
@@ -1087,13 +1760,13 @@
         <v>6</v>
       </c>
       <c r="G20">
-        <v>-7.6188229999999999</v>
+        <v>-7.618823</v>
       </c>
       <c r="H20">
         <v>109.138499</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>70</v>
       </c>
@@ -1110,7 +1783,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>80</v>
       </c>
@@ -1167,7 +1840,7 @@
         <v>6</v>
       </c>
       <c r="G24">
-        <v>-7.7898310000000004</v>
+        <v>-7.789831</v>
       </c>
       <c r="H24">
         <v>110.37488</v>
@@ -1190,7 +1863,7 @@
         <v>3</v>
       </c>
       <c r="G25">
-        <v>-7.5573550000000003</v>
+        <v>-7.557355</v>
       </c>
       <c r="H25">
         <v>110.815163</v>
@@ -1213,13 +1886,13 @@
         <v>6</v>
       </c>
       <c r="G26">
-        <v>-7.5571859999999997</v>
+        <v>-7.557186</v>
       </c>
       <c r="H26">
         <v>110.814977</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>73</v>
       </c>
@@ -1253,7 +1926,7 @@
         <v>3</v>
       </c>
       <c r="G28">
-        <v>-7.6183889999999996</v>
+        <v>-7.618389</v>
       </c>
       <c r="H28">
         <v>111.522891</v>
@@ -1276,13 +1949,13 @@
         <v>6</v>
       </c>
       <c r="G29">
-        <v>-7.6180219999999998</v>
+        <v>-7.618022</v>
       </c>
       <c r="H29">
         <v>111.528362</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>81</v>
       </c>
@@ -1316,7 +1989,7 @@
         <v>3</v>
       </c>
       <c r="G31">
-        <v>-7.2341790000000001</v>
+        <v>-7.234179</v>
       </c>
       <c r="H31">
         <v>112.754733</v>
@@ -1339,7 +2012,7 @@
         <v>6</v>
       </c>
       <c r="G32">
-        <v>-7.2361620000000002</v>
+        <v>-7.236162</v>
       </c>
       <c r="H32">
         <v>112.755821</v>
@@ -1362,10 +2035,10 @@
         <v>6</v>
       </c>
       <c r="G33">
-        <v>-7.2505480000000002</v>
+        <v>-7.250548</v>
       </c>
       <c r="H33">
-        <v>112.72839399999999</v>
+        <v>112.728394</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1385,10 +2058,10 @@
         <v>6</v>
       </c>
       <c r="G34">
-        <v>-7.2654269999999999</v>
+        <v>-7.265427</v>
       </c>
       <c r="H34">
-        <v>112.75227700000001</v>
+        <v>112.752277</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1408,10 +2081,10 @@
         <v>3</v>
       </c>
       <c r="G35">
-        <v>-7.9778180000000001</v>
+        <v>-7.977818</v>
       </c>
       <c r="H35">
-        <v>112.63740300000001</v>
+        <v>112.637403</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1431,7 +2104,7 @@
         <v>6</v>
       </c>
       <c r="G36">
-        <v>-7.9745720000000002</v>
+        <v>-7.974572</v>
       </c>
       <c r="H36">
         <v>112.63735</v>
@@ -1454,7 +2127,7 @@
         <v>6</v>
       </c>
       <c r="G37">
-        <v>-7.2346789999999999</v>
+        <v>-7.234679</v>
       </c>
       <c r="H37">
         <v>112.75712</v>
@@ -1477,7 +2150,7 @@
         <v>3</v>
       </c>
       <c r="G38">
-        <v>-8.1639149999999994</v>
+        <v>-8.163915</v>
       </c>
       <c r="H38">
         <v>113.702765</v>
@@ -1500,10 +2173,10 @@
         <v>6</v>
       </c>
       <c r="G39">
-        <v>-8.1378839999999997</v>
+        <v>-8.137884</v>
       </c>
       <c r="H39">
-        <v>114.39704999999999</v>
+        <v>114.39705</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1523,7 +2196,7 @@
         <v>3</v>
       </c>
       <c r="G40">
-        <v>3.5931730000000002</v>
+        <v>3.593173</v>
       </c>
       <c r="H40">
         <v>98.679209</v>
@@ -1546,13 +2219,13 @@
         <v>6</v>
       </c>
       <c r="G41">
-        <v>3.5931730000000002</v>
+        <v>3.593173</v>
       </c>
       <c r="H41">
         <v>98.679209</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:5">
       <c r="A42">
         <v>61</v>
       </c>
@@ -1569,7 +2242,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:5">
       <c r="A43">
         <v>62</v>
       </c>
@@ -1603,10 +2276,10 @@
         <v>3</v>
       </c>
       <c r="G44">
-        <v>-0.94310899999999998</v>
+        <v>-0.943109</v>
       </c>
       <c r="H44">
-        <v>100.37309999999999</v>
+        <v>100.3731</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1626,7 +2299,7 @@
         <v>6</v>
       </c>
       <c r="G45">
-        <v>-0.94121999999999995</v>
+        <v>-0.94122</v>
       </c>
       <c r="H45">
         <v>100.37309</v>
@@ -1652,7 +2325,7 @@
         <v>-3.022551</v>
       </c>
       <c r="H46">
-        <v>104.74742000000001</v>
+        <v>104.74742</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1672,7 +2345,7 @@
         <v>6</v>
       </c>
       <c r="G47">
-        <v>-3.0194549999999998</v>
+        <v>-3.019455</v>
       </c>
       <c r="H47">
         <v>104.75009</v>
@@ -1698,10 +2371,10 @@
         <v>-3.021862</v>
       </c>
       <c r="H48">
-        <v>104.74684000000001</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
+        <v>104.74684</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49">
         <v>55</v>
       </c>
@@ -1741,7 +2414,7 @@
         <v>103.798637</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:5">
       <c r="A51">
         <v>77</v>
       </c>
@@ -1775,7 +2448,7 @@
         <v>3</v>
       </c>
       <c r="G52">
-        <v>-6.2177379999999998</v>
+        <v>-6.217738</v>
       </c>
       <c r="H52">
         <v>106.861169</v>
@@ -1798,7 +2471,7 @@
         <v>3</v>
       </c>
       <c r="G53">
-        <v>-6.4164770000000004</v>
+        <v>-6.416477</v>
       </c>
       <c r="H53">
         <v>106.811902</v>
@@ -1821,13 +2494,13 @@
         <v>3</v>
       </c>
       <c r="G54">
-        <v>-6.5912009999999999</v>
+        <v>-6.591201</v>
       </c>
       <c r="H54">
         <v>106.791453</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:5">
       <c r="A55">
         <v>71</v>
       </c>
@@ -1861,7 +2534,7 @@
         <v>3</v>
       </c>
       <c r="G56">
-        <v>-5.5031020000000002</v>
+        <v>-5.503102</v>
       </c>
       <c r="H56">
         <v>105.336337</v>
@@ -1890,7 +2563,7 @@
         <v>105.261059</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:5">
       <c r="A58">
         <v>52</v>
       </c>
@@ -1907,26 +2580,26 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
-      <c r="A59">
+    <row r="59" s="1" customFormat="1" spans="1:8">
+      <c r="A59" s="1">
         <v>53</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D59" t="s">
-        <v>2</v>
-      </c>
-      <c r="E59" t="s">
-        <v>6</v>
-      </c>
-      <c r="G59">
-        <v>-5.2932300000000003</v>
-      </c>
-      <c r="H59">
+      <c r="D59" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G59" s="1">
+        <v>-5.29323</v>
+      </c>
+      <c r="H59" s="1">
         <v>105.18722</v>
       </c>
     </row>
@@ -1947,10 +2620,10 @@
         <v>6</v>
       </c>
       <c r="G60">
-        <v>-5.2941669999999998</v>
+        <v>-5.294167</v>
       </c>
       <c r="H60">
-        <v>105.18777799999999</v>
+        <v>105.187778</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -1976,24 +2649,24 @@
         <v>105.261059</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
-      <c r="A62">
+    <row r="62" s="1" customFormat="1" spans="1:5">
+      <c r="A62" s="1">
         <v>68</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D62" t="s">
-        <v>2</v>
-      </c>
-      <c r="E62" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8">
+      <c r="D62" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
       <c r="A63">
         <v>74</v>
       </c>
@@ -2010,7 +2683,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:5">
       <c r="A64">
         <v>76</v>
       </c>
@@ -2044,8 +2717,159 @@
         <v>3</v>
       </c>
     </row>
+    <row r="66" spans="1:5">
+      <c r="A66">
+        <v>79</v>
+      </c>
+      <c r="B66" t="s">
+        <v>16</v>
+      </c>
+      <c r="C66" t="s">
+        <v>89</v>
+      </c>
+      <c r="D66" t="s">
+        <v>2</v>
+      </c>
+      <c r="E66" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67">
+        <v>80</v>
+      </c>
+      <c r="B67" t="s">
+        <v>31</v>
+      </c>
+      <c r="C67" t="s">
+        <v>90</v>
+      </c>
+      <c r="D67" t="s">
+        <v>2</v>
+      </c>
+      <c r="E67" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68">
+        <v>81</v>
+      </c>
+      <c r="B68" t="s">
+        <v>58</v>
+      </c>
+      <c r="C68" t="s">
+        <v>91</v>
+      </c>
+      <c r="D68" t="s">
+        <v>2</v>
+      </c>
+      <c r="E68" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69">
+        <v>82</v>
+      </c>
+      <c r="B69" t="s">
+        <v>61</v>
+      </c>
+      <c r="C69" t="s">
+        <v>92</v>
+      </c>
+      <c r="D69" t="s">
+        <v>2</v>
+      </c>
+      <c r="E69" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70">
+        <v>83</v>
+      </c>
+      <c r="B70" t="s">
+        <v>61</v>
+      </c>
+      <c r="C70" t="s">
+        <v>93</v>
+      </c>
+      <c r="D70" t="s">
+        <v>2</v>
+      </c>
+      <c r="E70" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A2:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="1"/>
+  <cols>
+    <col min="2" max="2" width="23.8571428571429" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2">
+      <c r="B2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>